<commit_message>
Artefatos OK no QA
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-BRAgendamentoRegulacaoAssistencial.xlsx
+++ b/docs/StructureDefinition-BRAgendamentoRegulacaoAssistencial.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -72,7 +72,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>null (http://www.saude.gov.br)</t>
   </si>
   <si>
     <t>Jurisdiction</t>
@@ -281,6 +281,9 @@
     <t>Appointment.id</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
@@ -298,9 +301,6 @@
   </si>
   <si>
     <t>Resource.id</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>Appointment.meta</t>
@@ -2130,17 +2130,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="73.1796875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="51.86328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="21.76171875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="70.625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="49.90234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="21.19140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="37.5859375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.9296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.47265625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.87890625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.2734375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.7265625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="91.46875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="86.76171875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2149,27 +2149,27 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="38.8125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="95.56640625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="80.3515625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.171875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="36.22265625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.4609375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.86328125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="91.51171875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="76.33984375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.52734375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="21.13671875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="38.34375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="15.06640625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.421875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="32.73046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.28515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.6875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="33.4765625" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="106.0703125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="151.71484375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="75.30859375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="32.03515625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="100.66015625" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="145.0859375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="32.4453125" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="71.80078125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2428,7 +2428,7 @@
         <v>78</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H3" t="s" s="2">
         <v>77</v>
@@ -2437,19 +2437,19 @@
         <v>77</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N3" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
@@ -2499,13 +2499,13 @@
         <v>77</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI3" t="s" s="2">
         <v>77</v>
@@ -2545,7 +2545,7 @@
         <v>78</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s" s="2">
         <v>77</v>
@@ -2554,7 +2554,7 @@
         <v>77</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K4" t="s" s="2">
         <v>96</v>
@@ -2620,7 +2620,7 @@
         <v>78</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI4" t="s" s="2">
         <v>77</v>
@@ -2666,10 +2666,10 @@
         <v>77</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K5" t="s" s="2">
         <v>102</v>
@@ -2737,7 +2737,7 @@
         <v>78</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI5" t="s" s="2">
         <v>77</v>
@@ -2854,7 +2854,7 @@
         <v>78</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI6" t="s" s="2">
         <v>77</v>
@@ -2894,7 +2894,7 @@
         <v>78</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H7" t="s" s="2">
         <v>77</v>
@@ -2971,7 +2971,7 @@
         <v>78</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI7" t="s" s="2">
         <v>77</v>
@@ -3251,7 +3251,7 @@
         <v>77</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J10" t="s" s="2">
         <v>77</v>
@@ -3373,7 +3373,7 @@
         <v>77</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K11" t="s" s="2">
         <v>146</v>
@@ -3476,19 +3476,19 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>77</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K12" t="s" s="2">
         <v>108</v>
@@ -3553,10 +3553,10 @@
         <v>154</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI12" t="s" s="2">
         <v>77</v>
@@ -3605,7 +3605,7 @@
         <v>77</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K13" t="s" s="2">
         <v>167</v>
@@ -3669,7 +3669,7 @@
         <v>78</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI13" t="s" s="2">
         <v>77</v>
@@ -3706,10 +3706,10 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>77</v>
@@ -3718,7 +3718,7 @@
         <v>77</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K14" t="s" s="2">
         <v>167</v>
@@ -3824,7 +3824,7 @@
         <v>78</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>77</v>
@@ -3899,7 +3899,7 @@
         <v>78</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>77</v>
@@ -4053,10 +4053,10 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>77</v>
@@ -4065,7 +4065,7 @@
         <v>77</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K17" t="s" s="2">
         <v>192</v>
@@ -4175,7 +4175,7 @@
         <v>78</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>77</v>
@@ -4250,7 +4250,7 @@
         <v>78</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI18" t="s" s="2">
         <v>77</v>
@@ -4404,10 +4404,10 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>77</v>
@@ -4416,7 +4416,7 @@
         <v>77</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K20" t="s" s="2">
         <v>102</v>
@@ -4486,7 +4486,7 @@
         <v>78</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI20" t="s" s="2">
         <v>77</v>
@@ -4526,7 +4526,7 @@
         <v>78</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>77</v>
@@ -4535,7 +4535,7 @@
         <v>77</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K21" t="s" s="2">
         <v>181</v>
@@ -4603,7 +4603,7 @@
         <v>78</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI21" t="s" s="2">
         <v>77</v>
@@ -4640,10 +4640,10 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>77</v>
@@ -4652,7 +4652,7 @@
         <v>77</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K22" t="s" s="2">
         <v>108</v>
@@ -4720,7 +4720,7 @@
         <v>78</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>77</v>
@@ -4760,7 +4760,7 @@
         <v>78</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>77</v>
@@ -4769,7 +4769,7 @@
         <v>77</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K23" t="s" s="2">
         <v>181</v>
@@ -4837,7 +4837,7 @@
         <v>78</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>77</v>
@@ -4877,7 +4877,7 @@
         <v>78</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>77</v>
@@ -4886,7 +4886,7 @@
         <v>77</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K24" t="s" s="2">
         <v>232</v>
@@ -4956,7 +4956,7 @@
         <v>78</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>77</v>
@@ -5005,7 +5005,7 @@
         <v>77</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K25" t="s" s="2">
         <v>181</v>
@@ -5075,7 +5075,7 @@
         <v>78</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>77</v>
@@ -5112,10 +5112,10 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>77</v>
@@ -5124,7 +5124,7 @@
         <v>77</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K26" t="s" s="2">
         <v>167</v>
@@ -5232,7 +5232,7 @@
         <v>78</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>77</v>
@@ -5307,7 +5307,7 @@
         <v>78</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>77</v>
@@ -5461,10 +5461,10 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>77</v>
@@ -5473,7 +5473,7 @@
         <v>77</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K29" t="s" s="2">
         <v>192</v>
@@ -5583,7 +5583,7 @@
         <v>78</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>77</v>
@@ -5658,7 +5658,7 @@
         <v>78</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>77</v>
@@ -5812,10 +5812,10 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>77</v>
@@ -5824,7 +5824,7 @@
         <v>77</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K32" t="s" s="2">
         <v>102</v>
@@ -5894,7 +5894,7 @@
         <v>78</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI32" t="s" s="2">
         <v>77</v>
@@ -5934,7 +5934,7 @@
         <v>78</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>77</v>
@@ -5943,7 +5943,7 @@
         <v>77</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K33" t="s" s="2">
         <v>181</v>
@@ -6011,7 +6011,7 @@
         <v>78</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>77</v>
@@ -6048,10 +6048,10 @@
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>77</v>
@@ -6060,7 +6060,7 @@
         <v>77</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K34" t="s" s="2">
         <v>108</v>
@@ -6128,7 +6128,7 @@
         <v>78</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>77</v>
@@ -6168,7 +6168,7 @@
         <v>78</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>77</v>
@@ -6177,7 +6177,7 @@
         <v>77</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K35" t="s" s="2">
         <v>181</v>
@@ -6245,7 +6245,7 @@
         <v>78</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>77</v>
@@ -6285,7 +6285,7 @@
         <v>78</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>77</v>
@@ -6294,7 +6294,7 @@
         <v>77</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K36" t="s" s="2">
         <v>232</v>
@@ -6364,7 +6364,7 @@
         <v>78</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>77</v>
@@ -6413,7 +6413,7 @@
         <v>77</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K37" t="s" s="2">
         <v>181</v>
@@ -6483,7 +6483,7 @@
         <v>78</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>77</v>
@@ -6523,7 +6523,7 @@
         <v>78</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>77</v>
@@ -6532,7 +6532,7 @@
         <v>77</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K38" t="s" s="2">
         <v>167</v>
@@ -6638,7 +6638,7 @@
         <v>78</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>77</v>
@@ -6713,7 +6713,7 @@
         <v>78</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>77</v>
@@ -6867,10 +6867,10 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>77</v>
@@ -6879,7 +6879,7 @@
         <v>77</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K41" t="s" s="2">
         <v>192</v>
@@ -6989,7 +6989,7 @@
         <v>78</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>77</v>
@@ -7064,7 +7064,7 @@
         <v>78</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>77</v>
@@ -7218,10 +7218,10 @@
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>77</v>
@@ -7230,7 +7230,7 @@
         <v>77</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K44" t="s" s="2">
         <v>102</v>
@@ -7300,7 +7300,7 @@
         <v>78</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI44" t="s" s="2">
         <v>77</v>
@@ -7340,7 +7340,7 @@
         <v>78</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>77</v>
@@ -7349,7 +7349,7 @@
         <v>77</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K45" t="s" s="2">
         <v>181</v>
@@ -7417,7 +7417,7 @@
         <v>78</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>77</v>
@@ -7454,10 +7454,10 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>77</v>
@@ -7466,7 +7466,7 @@
         <v>77</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K46" t="s" s="2">
         <v>108</v>
@@ -7534,7 +7534,7 @@
         <v>78</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>77</v>
@@ -7574,7 +7574,7 @@
         <v>78</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>77</v>
@@ -7583,7 +7583,7 @@
         <v>77</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K47" t="s" s="2">
         <v>181</v>
@@ -7651,7 +7651,7 @@
         <v>78</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>77</v>
@@ -7691,7 +7691,7 @@
         <v>78</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>77</v>
@@ -7700,7 +7700,7 @@
         <v>77</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K48" t="s" s="2">
         <v>232</v>
@@ -7770,7 +7770,7 @@
         <v>78</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>77</v>
@@ -7819,7 +7819,7 @@
         <v>77</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K49" t="s" s="2">
         <v>181</v>
@@ -7889,7 +7889,7 @@
         <v>78</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>77</v>
@@ -7926,10 +7926,10 @@
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>77</v>
@@ -7938,7 +7938,7 @@
         <v>77</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K50" t="s" s="2">
         <v>167</v>
@@ -8004,7 +8004,7 @@
         <v>78</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>77</v>
@@ -8044,7 +8044,7 @@
         <v>78</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>77</v>
@@ -8119,7 +8119,7 @@
         <v>78</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>77</v>
@@ -8273,10 +8273,10 @@
       </c>
       <c r="E53" s="2"/>
       <c r="F53" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H53" t="s" s="2">
         <v>77</v>
@@ -8285,7 +8285,7 @@
         <v>77</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K53" t="s" s="2">
         <v>192</v>
@@ -8395,7 +8395,7 @@
         <v>78</v>
       </c>
       <c r="G54" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H54" t="s" s="2">
         <v>77</v>
@@ -8470,7 +8470,7 @@
         <v>78</v>
       </c>
       <c r="AH54" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI54" t="s" s="2">
         <v>77</v>
@@ -8624,10 +8624,10 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G56" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H56" t="s" s="2">
         <v>77</v>
@@ -8636,7 +8636,7 @@
         <v>77</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K56" t="s" s="2">
         <v>102</v>
@@ -8706,7 +8706,7 @@
         <v>78</v>
       </c>
       <c r="AH56" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI56" t="s" s="2">
         <v>77</v>
@@ -8746,7 +8746,7 @@
         <v>78</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H57" t="s" s="2">
         <v>77</v>
@@ -8755,7 +8755,7 @@
         <v>77</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K57" t="s" s="2">
         <v>181</v>
@@ -8823,7 +8823,7 @@
         <v>78</v>
       </c>
       <c r="AH57" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI57" t="s" s="2">
         <v>77</v>
@@ -8860,10 +8860,10 @@
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>77</v>
@@ -8872,7 +8872,7 @@
         <v>77</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K58" t="s" s="2">
         <v>108</v>
@@ -8940,7 +8940,7 @@
         <v>78</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>77</v>
@@ -8980,7 +8980,7 @@
         <v>78</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>77</v>
@@ -8989,7 +8989,7 @@
         <v>77</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K59" t="s" s="2">
         <v>181</v>
@@ -9057,7 +9057,7 @@
         <v>78</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>77</v>
@@ -9097,7 +9097,7 @@
         <v>78</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H60" t="s" s="2">
         <v>77</v>
@@ -9106,7 +9106,7 @@
         <v>77</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K60" t="s" s="2">
         <v>232</v>
@@ -9176,7 +9176,7 @@
         <v>78</v>
       </c>
       <c r="AH60" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI60" t="s" s="2">
         <v>77</v>
@@ -9225,7 +9225,7 @@
         <v>77</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K61" t="s" s="2">
         <v>181</v>
@@ -9295,7 +9295,7 @@
         <v>78</v>
       </c>
       <c r="AH61" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI61" t="s" s="2">
         <v>77</v>
@@ -9344,7 +9344,7 @@
         <v>77</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K62" t="s" s="2">
         <v>167</v>
@@ -9447,10 +9447,10 @@
       </c>
       <c r="E63" s="2"/>
       <c r="F63" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G63" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H63" t="s" s="2">
         <v>77</v>
@@ -9640,7 +9640,7 @@
         <v>78</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI64" t="s" s="2">
         <v>77</v>
@@ -9794,10 +9794,10 @@
       </c>
       <c r="E66" s="2"/>
       <c r="F66" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G66" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H66" t="s" s="2">
         <v>77</v>
@@ -9806,7 +9806,7 @@
         <v>77</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K66" t="s" s="2">
         <v>181</v>
@@ -9874,7 +9874,7 @@
         <v>78</v>
       </c>
       <c r="AH66" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI66" t="s" s="2">
         <v>324</v>
@@ -9923,7 +9923,7 @@
         <v>77</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K67" t="s" s="2">
         <v>102</v>
@@ -9991,7 +9991,7 @@
         <v>78</v>
       </c>
       <c r="AH67" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI67" t="s" s="2">
         <v>77</v>
@@ -10040,7 +10040,7 @@
         <v>77</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K68" t="s" s="2">
         <v>146</v>
@@ -10108,7 +10108,7 @@
         <v>78</v>
       </c>
       <c r="AH68" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI68" t="s" s="2">
         <v>77</v>
@@ -10157,7 +10157,7 @@
         <v>77</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K69" t="s" s="2">
         <v>181</v>
@@ -10225,7 +10225,7 @@
         <v>78</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>77</v>
@@ -10342,7 +10342,7 @@
         <v>78</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI70" t="s" s="2">
         <v>77</v>
@@ -10457,7 +10457,7 @@
         <v>78</v>
       </c>
       <c r="AH71" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI71" t="s" s="2">
         <v>77</v>
@@ -10497,7 +10497,7 @@
         <v>78</v>
       </c>
       <c r="G72" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H72" t="s" s="2">
         <v>77</v>
@@ -10685,7 +10685,7 @@
         <v>78</v>
       </c>
       <c r="AH73" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI73" t="s" s="2">
         <v>77</v>
@@ -10842,7 +10842,7 @@
         <v>78</v>
       </c>
       <c r="G75" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H75" t="s" s="2">
         <v>77</v>
@@ -10851,7 +10851,7 @@
         <v>77</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K75" t="s" s="2">
         <v>181</v>
@@ -10919,7 +10919,7 @@
         <v>78</v>
       </c>
       <c r="AH75" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI75" t="s" s="2">
         <v>324</v>
@@ -10968,7 +10968,7 @@
         <v>77</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K76" t="s" s="2">
         <v>102</v>
@@ -11036,7 +11036,7 @@
         <v>78</v>
       </c>
       <c r="AH76" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI76" t="s" s="2">
         <v>77</v>
@@ -11076,7 +11076,7 @@
         <v>78</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H77" t="s" s="2">
         <v>77</v>
@@ -11085,7 +11085,7 @@
         <v>77</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K77" t="s" s="2">
         <v>146</v>
@@ -11153,7 +11153,7 @@
         <v>78</v>
       </c>
       <c r="AH77" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI77" t="s" s="2">
         <v>77</v>
@@ -11268,7 +11268,7 @@
         <v>78</v>
       </c>
       <c r="AH78" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI78" t="s" s="2">
         <v>77</v>
@@ -11431,10 +11431,10 @@
         <v>77</v>
       </c>
       <c r="I80" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K80" t="s" s="2">
         <v>108</v>
@@ -11504,7 +11504,7 @@
         <v>78</v>
       </c>
       <c r="AH80" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI80" t="s" s="2">
         <v>77</v>
@@ -11553,7 +11553,7 @@
         <v>77</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K81" t="s" s="2">
         <v>167</v>
@@ -11623,7 +11623,7 @@
         <v>78</v>
       </c>
       <c r="AH81" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI81" t="s" s="2">
         <v>77</v>
@@ -11663,7 +11663,7 @@
         <v>78</v>
       </c>
       <c r="G82" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H82" t="s" s="2">
         <v>77</v>
@@ -11672,7 +11672,7 @@
         <v>77</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K82" t="s" s="2">
         <v>102</v>
@@ -11742,7 +11742,7 @@
         <v>78</v>
       </c>
       <c r="AH82" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI82" t="s" s="2">
         <v>77</v>
@@ -11782,7 +11782,7 @@
         <v>78</v>
       </c>
       <c r="G83" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H83" t="s" s="2">
         <v>77</v>
@@ -11791,7 +11791,7 @@
         <v>77</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K83" t="s" s="2">
         <v>181</v>
@@ -11859,7 +11859,7 @@
         <v>78</v>
       </c>
       <c r="AH83" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI83" t="s" s="2">
         <v>77</v>
@@ -11908,7 +11908,7 @@
         <v>77</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K84" t="s" s="2">
         <v>411</v>
@@ -11974,7 +11974,7 @@
         <v>78</v>
       </c>
       <c r="AH84" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI84" t="s" s="2">
         <v>77</v>
@@ -12023,7 +12023,7 @@
         <v>77</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K85" t="s" s="2">
         <v>418</v>
@@ -12091,7 +12091,7 @@
         <v>78</v>
       </c>
       <c r="AH85" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI85" t="s" s="2">
         <v>77</v>
@@ -12140,7 +12140,7 @@
         <v>77</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K86" t="s" s="2">
         <v>181</v>
@@ -12208,7 +12208,7 @@
         <v>78</v>
       </c>
       <c r="AH86" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI86" t="s" s="2">
         <v>77</v>
@@ -12250,7 +12250,7 @@
         <v>78</v>
       </c>
       <c r="G87" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H87" t="s" s="2">
         <v>77</v>
@@ -12440,7 +12440,7 @@
         <v>78</v>
       </c>
       <c r="AH88" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI88" t="s" s="2">
         <v>77</v>
@@ -12597,7 +12597,7 @@
         <v>78</v>
       </c>
       <c r="G90" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H90" t="s" s="2">
         <v>77</v>
@@ -12606,7 +12606,7 @@
         <v>77</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K90" t="s" s="2">
         <v>181</v>
@@ -12674,7 +12674,7 @@
         <v>78</v>
       </c>
       <c r="AH90" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI90" t="s" s="2">
         <v>324</v>
@@ -12723,7 +12723,7 @@
         <v>77</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K91" t="s" s="2">
         <v>102</v>
@@ -12791,7 +12791,7 @@
         <v>78</v>
       </c>
       <c r="AH91" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI91" t="s" s="2">
         <v>77</v>
@@ -12831,7 +12831,7 @@
         <v>78</v>
       </c>
       <c r="G92" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H92" t="s" s="2">
         <v>77</v>
@@ -12840,7 +12840,7 @@
         <v>77</v>
       </c>
       <c r="J92" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K92" t="s" s="2">
         <v>146</v>
@@ -12908,7 +12908,7 @@
         <v>78</v>
       </c>
       <c r="AH92" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI92" t="s" s="2">
         <v>77</v>
@@ -13023,7 +13023,7 @@
         <v>78</v>
       </c>
       <c r="AH93" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI93" t="s" s="2">
         <v>77</v>
@@ -13186,10 +13186,10 @@
         <v>77</v>
       </c>
       <c r="I95" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J95" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K95" t="s" s="2">
         <v>108</v>
@@ -13259,7 +13259,7 @@
         <v>78</v>
       </c>
       <c r="AH95" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI95" t="s" s="2">
         <v>77</v>
@@ -13308,7 +13308,7 @@
         <v>77</v>
       </c>
       <c r="J96" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K96" t="s" s="2">
         <v>167</v>
@@ -13378,7 +13378,7 @@
         <v>78</v>
       </c>
       <c r="AH96" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI96" t="s" s="2">
         <v>77</v>
@@ -13418,7 +13418,7 @@
         <v>78</v>
       </c>
       <c r="G97" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H97" t="s" s="2">
         <v>77</v>
@@ -13427,7 +13427,7 @@
         <v>77</v>
       </c>
       <c r="J97" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K97" t="s" s="2">
         <v>102</v>
@@ -13497,7 +13497,7 @@
         <v>78</v>
       </c>
       <c r="AH97" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI97" t="s" s="2">
         <v>77</v>
@@ -13537,7 +13537,7 @@
         <v>78</v>
       </c>
       <c r="G98" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H98" t="s" s="2">
         <v>77</v>
@@ -13546,7 +13546,7 @@
         <v>77</v>
       </c>
       <c r="J98" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K98" t="s" s="2">
         <v>181</v>
@@ -13614,7 +13614,7 @@
         <v>78</v>
       </c>
       <c r="AH98" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI98" t="s" s="2">
         <v>77</v>
@@ -13663,7 +13663,7 @@
         <v>77</v>
       </c>
       <c r="J99" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K99" t="s" s="2">
         <v>411</v>
@@ -13729,7 +13729,7 @@
         <v>78</v>
       </c>
       <c r="AH99" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI99" t="s" s="2">
         <v>77</v>
@@ -13778,7 +13778,7 @@
         <v>77</v>
       </c>
       <c r="J100" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K100" t="s" s="2">
         <v>418</v>
@@ -13846,7 +13846,7 @@
         <v>78</v>
       </c>
       <c r="AH100" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI100" t="s" s="2">
         <v>77</v>
@@ -13895,7 +13895,7 @@
         <v>77</v>
       </c>
       <c r="J101" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K101" t="s" s="2">
         <v>181</v>
@@ -13963,7 +13963,7 @@
         <v>78</v>
       </c>
       <c r="AH101" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI101" t="s" s="2">
         <v>77</v>
@@ -14003,7 +14003,7 @@
         <v>78</v>
       </c>
       <c r="G102" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H102" t="s" s="2">
         <v>77</v>
@@ -14012,7 +14012,7 @@
         <v>77</v>
       </c>
       <c r="J102" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K102" t="s" s="2">
         <v>445</v>
@@ -14078,7 +14078,7 @@
         <v>78</v>
       </c>
       <c r="AH102" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI102" t="s" s="2">
         <v>77</v>
@@ -14118,7 +14118,7 @@
         <v>78</v>
       </c>
       <c r="G103" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H103" t="s" s="2">
         <v>77</v>
@@ -14127,7 +14127,7 @@
         <v>77</v>
       </c>
       <c r="J103" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K103" t="s" s="2">
         <v>445</v>
@@ -14193,7 +14193,7 @@
         <v>78</v>
       </c>
       <c r="AH103" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI103" t="s" s="2">
         <v>77</v>
@@ -14308,7 +14308,7 @@
         <v>78</v>
       </c>
       <c r="AH104" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI104" t="s" s="2">
         <v>77</v>
@@ -14463,7 +14463,7 @@
         <v>78</v>
       </c>
       <c r="G106" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H106" t="s" s="2">
         <v>77</v>
@@ -14540,7 +14540,7 @@
         <v>78</v>
       </c>
       <c r="AH106" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI106" t="s" s="2">
         <v>77</v>
@@ -14657,7 +14657,7 @@
         <v>78</v>
       </c>
       <c r="AH107" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI107" t="s" s="2">
         <v>77</v>
@@ -14772,7 +14772,7 @@
         <v>78</v>
       </c>
       <c r="AH108" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI108" t="s" s="2">
         <v>77</v>
@@ -14809,10 +14809,10 @@
       </c>
       <c r="E109" s="2"/>
       <c r="F109" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G109" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H109" t="s" s="2">
         <v>77</v>
@@ -15002,7 +15002,7 @@
         <v>78</v>
       </c>
       <c r="AH110" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI110" t="s" s="2">
         <v>77</v>
@@ -15156,10 +15156,10 @@
       </c>
       <c r="E112" s="2"/>
       <c r="F112" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G112" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H112" t="s" s="2">
         <v>77</v>
@@ -15168,7 +15168,7 @@
         <v>77</v>
       </c>
       <c r="J112" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K112" t="s" s="2">
         <v>181</v>
@@ -15236,7 +15236,7 @@
         <v>78</v>
       </c>
       <c r="AH112" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI112" t="s" s="2">
         <v>324</v>
@@ -15285,7 +15285,7 @@
         <v>77</v>
       </c>
       <c r="J113" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K113" t="s" s="2">
         <v>102</v>
@@ -15353,7 +15353,7 @@
         <v>78</v>
       </c>
       <c r="AH113" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI113" t="s" s="2">
         <v>77</v>
@@ -15402,7 +15402,7 @@
         <v>77</v>
       </c>
       <c r="J114" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K114" t="s" s="2">
         <v>146</v>
@@ -15470,7 +15470,7 @@
         <v>78</v>
       </c>
       <c r="AH114" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI114" t="s" s="2">
         <v>77</v>
@@ -15519,7 +15519,7 @@
         <v>77</v>
       </c>
       <c r="J115" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K115" t="s" s="2">
         <v>181</v>
@@ -15587,7 +15587,7 @@
         <v>78</v>
       </c>
       <c r="AH115" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI115" t="s" s="2">
         <v>77</v>
@@ -15624,10 +15624,10 @@
       </c>
       <c r="E116" s="2"/>
       <c r="F116" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G116" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H116" t="s" s="2">
         <v>77</v>
@@ -15699,7 +15699,7 @@
         <v>503</v>
       </c>
       <c r="AG116" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AH116" t="s" s="2">
         <v>79</v>
@@ -15817,7 +15817,7 @@
         <v>78</v>
       </c>
       <c r="AH117" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI117" t="s" s="2">
         <v>77</v>
@@ -15980,10 +15980,10 @@
         <v>77</v>
       </c>
       <c r="I119" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J119" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K119" t="s" s="2">
         <v>134</v>
@@ -16090,10 +16090,10 @@
       </c>
       <c r="E120" s="2"/>
       <c r="F120" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G120" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H120" t="s" s="2">
         <v>77</v>
@@ -16102,7 +16102,7 @@
         <v>77</v>
       </c>
       <c r="J120" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K120" t="s" s="2">
         <v>167</v>
@@ -16285,7 +16285,7 @@
         <v>78</v>
       </c>
       <c r="AH121" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI121" t="s" s="2">
         <v>77</v>
@@ -16439,10 +16439,10 @@
       </c>
       <c r="E123" s="2"/>
       <c r="F123" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G123" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H123" t="s" s="2">
         <v>77</v>
@@ -16451,7 +16451,7 @@
         <v>77</v>
       </c>
       <c r="J123" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K123" t="s" s="2">
         <v>192</v>
@@ -16636,7 +16636,7 @@
         <v>78</v>
       </c>
       <c r="AH124" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI124" t="s" s="2">
         <v>77</v>
@@ -16790,10 +16790,10 @@
       </c>
       <c r="E126" s="2"/>
       <c r="F126" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G126" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H126" t="s" s="2">
         <v>77</v>
@@ -16802,7 +16802,7 @@
         <v>77</v>
       </c>
       <c r="J126" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K126" t="s" s="2">
         <v>102</v>
@@ -16872,7 +16872,7 @@
         <v>78</v>
       </c>
       <c r="AH126" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI126" t="s" s="2">
         <v>77</v>
@@ -16912,7 +16912,7 @@
         <v>78</v>
       </c>
       <c r="G127" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H127" t="s" s="2">
         <v>77</v>
@@ -16921,7 +16921,7 @@
         <v>77</v>
       </c>
       <c r="J127" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K127" t="s" s="2">
         <v>181</v>
@@ -16989,7 +16989,7 @@
         <v>78</v>
       </c>
       <c r="AH127" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI127" t="s" s="2">
         <v>77</v>
@@ -17026,10 +17026,10 @@
       </c>
       <c r="E128" s="2"/>
       <c r="F128" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G128" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H128" t="s" s="2">
         <v>77</v>
@@ -17038,7 +17038,7 @@
         <v>77</v>
       </c>
       <c r="J128" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K128" t="s" s="2">
         <v>108</v>
@@ -17106,7 +17106,7 @@
         <v>78</v>
       </c>
       <c r="AH128" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI128" t="s" s="2">
         <v>77</v>
@@ -17146,7 +17146,7 @@
         <v>78</v>
       </c>
       <c r="G129" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H129" t="s" s="2">
         <v>77</v>
@@ -17155,7 +17155,7 @@
         <v>77</v>
       </c>
       <c r="J129" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K129" t="s" s="2">
         <v>181</v>
@@ -17223,7 +17223,7 @@
         <v>78</v>
       </c>
       <c r="AH129" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI129" t="s" s="2">
         <v>77</v>
@@ -17272,7 +17272,7 @@
         <v>77</v>
       </c>
       <c r="J130" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K130" t="s" s="2">
         <v>232</v>
@@ -17342,7 +17342,7 @@
         <v>78</v>
       </c>
       <c r="AH130" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI130" t="s" s="2">
         <v>77</v>
@@ -17391,7 +17391,7 @@
         <v>77</v>
       </c>
       <c r="J131" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K131" t="s" s="2">
         <v>181</v>
@@ -17461,7 +17461,7 @@
         <v>78</v>
       </c>
       <c r="AH131" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI131" t="s" s="2">
         <v>77</v>
@@ -17498,10 +17498,10 @@
       </c>
       <c r="E132" s="2"/>
       <c r="F132" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G132" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H132" t="s" s="2">
         <v>77</v>
@@ -17510,7 +17510,7 @@
         <v>77</v>
       </c>
       <c r="J132" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K132" t="s" s="2">
         <v>539</v>
@@ -17576,7 +17576,7 @@
         <v>78</v>
       </c>
       <c r="AH132" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI132" t="s" s="2">
         <v>77</v>
@@ -17691,7 +17691,7 @@
         <v>78</v>
       </c>
       <c r="AH133" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI133" t="s" s="2">
         <v>77</v>
@@ -17857,7 +17857,7 @@
         <v>77</v>
       </c>
       <c r="J135" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K135" t="s" s="2">
         <v>181</v>
@@ -17925,7 +17925,7 @@
         <v>78</v>
       </c>
       <c r="AH135" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI135" t="s" s="2">
         <v>324</v>
@@ -17974,7 +17974,7 @@
         <v>77</v>
       </c>
       <c r="J136" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K136" t="s" s="2">
         <v>102</v>
@@ -18042,7 +18042,7 @@
         <v>78</v>
       </c>
       <c r="AH136" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI136" t="s" s="2">
         <v>77</v>
@@ -18079,10 +18079,10 @@
       </c>
       <c r="E137" s="2"/>
       <c r="F137" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G137" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H137" t="s" s="2">
         <v>77</v>
@@ -18091,7 +18091,7 @@
         <v>77</v>
       </c>
       <c r="J137" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K137" t="s" s="2">
         <v>146</v>
@@ -18159,7 +18159,7 @@
         <v>78</v>
       </c>
       <c r="AH137" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI137" t="s" s="2">
         <v>77</v>
@@ -18274,7 +18274,7 @@
         <v>78</v>
       </c>
       <c r="AH138" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI138" t="s" s="2">
         <v>77</v>
@@ -18437,10 +18437,10 @@
         <v>77</v>
       </c>
       <c r="I140" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J140" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K140" t="s" s="2">
         <v>108</v>
@@ -18510,7 +18510,7 @@
         <v>78</v>
       </c>
       <c r="AH140" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI140" t="s" s="2">
         <v>77</v>
@@ -18559,7 +18559,7 @@
         <v>77</v>
       </c>
       <c r="J141" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K141" t="s" s="2">
         <v>167</v>
@@ -18629,7 +18629,7 @@
         <v>78</v>
       </c>
       <c r="AH141" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI141" t="s" s="2">
         <v>77</v>
@@ -18666,10 +18666,10 @@
       </c>
       <c r="E142" s="2"/>
       <c r="F142" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G142" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H142" t="s" s="2">
         <v>77</v>
@@ -18678,7 +18678,7 @@
         <v>77</v>
       </c>
       <c r="J142" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K142" t="s" s="2">
         <v>102</v>
@@ -18748,7 +18748,7 @@
         <v>78</v>
       </c>
       <c r="AH142" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI142" t="s" s="2">
         <v>77</v>
@@ -18785,10 +18785,10 @@
       </c>
       <c r="E143" s="2"/>
       <c r="F143" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G143" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H143" t="s" s="2">
         <v>77</v>
@@ -18797,7 +18797,7 @@
         <v>77</v>
       </c>
       <c r="J143" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K143" t="s" s="2">
         <v>181</v>
@@ -18865,7 +18865,7 @@
         <v>78</v>
       </c>
       <c r="AH143" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI143" t="s" s="2">
         <v>77</v>
@@ -18914,7 +18914,7 @@
         <v>77</v>
       </c>
       <c r="J144" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K144" t="s" s="2">
         <v>411</v>
@@ -18980,7 +18980,7 @@
         <v>78</v>
       </c>
       <c r="AH144" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI144" t="s" s="2">
         <v>77</v>
@@ -19029,7 +19029,7 @@
         <v>77</v>
       </c>
       <c r="J145" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K145" t="s" s="2">
         <v>418</v>
@@ -19097,7 +19097,7 @@
         <v>78</v>
       </c>
       <c r="AH145" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI145" t="s" s="2">
         <v>77</v>
@@ -19146,7 +19146,7 @@
         <v>77</v>
       </c>
       <c r="J146" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K146" t="s" s="2">
         <v>181</v>
@@ -19214,7 +19214,7 @@
         <v>78</v>
       </c>
       <c r="AH146" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI146" t="s" s="2">
         <v>77</v>
@@ -19263,7 +19263,7 @@
         <v>77</v>
       </c>
       <c r="J147" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K147" t="s" s="2">
         <v>108</v>
@@ -19329,7 +19329,7 @@
         <v>78</v>
       </c>
       <c r="AH147" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI147" t="s" s="2">
         <v>77</v>
@@ -19366,10 +19366,10 @@
       </c>
       <c r="E148" s="2"/>
       <c r="F148" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G148" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H148" t="s" s="2">
         <v>77</v>
@@ -19378,7 +19378,7 @@
         <v>77</v>
       </c>
       <c r="J148" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K148" t="s" s="2">
         <v>108</v>
@@ -19441,10 +19441,10 @@
         <v>567</v>
       </c>
       <c r="AG148" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AH148" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI148" t="s" s="2">
         <v>77</v>
@@ -19559,7 +19559,7 @@
         <v>78</v>
       </c>
       <c r="AH149" t="s" s="2">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AI149" t="s" s="2">
         <v>77</v>

</xml_diff>